<commit_message>
update user case acessórios
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
+++ b/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/DSS/Configura-Facil/diagramas/UseCases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871598C6-894A-E542-8F38-526CA6B67577}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20A2C50-6DAF-C34B-B48C-2112B394C11F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>System response</t>
   </si>
@@ -67,15 +67,9 @@
     <t>1. Informa cancelamento do componente</t>
   </si>
   <si>
-    <t>6. Confirma componte</t>
-  </si>
-  <si>
     <t>4. Verifica necessidade de componentes extras</t>
   </si>
   <si>
-    <t>7. Adiciona componente</t>
-  </si>
-  <si>
     <t>5.3. Retira componentes incompatíveis</t>
   </si>
   <si>
@@ -106,10 +100,25 @@
     <t xml:space="preserve"> Alternativa 2 [Necessita mais componentes] Passo 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Excepção 3 [Cliente não aceita componente] Passos 4.2, 5.2 e 6</t>
-  </si>
-  <si>
     <t>Componente acessório selecionado</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>3. Apresenta preço do componente</t>
+  </si>
+  <si>
+    <t>6. Apresenta preço final</t>
+  </si>
+  <si>
+    <t>7. Confirma componte</t>
+  </si>
+  <si>
+    <t>8.  Adiciona componente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Excepção 3 [Cliente não aceita componente] Passos 4.2, 5.2 e 7</t>
   </si>
 </sst>
 </file>
@@ -394,6 +403,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -403,6 +413,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -412,28 +443,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D25"/>
+  <dimension ref="B1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,45 +771,45 @@
     <col min="4" max="4" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="C5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -810,141 +819,153 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+    <row r="7" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+    <row r="8" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+    <row r="9" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="24"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="5" t="s">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="14"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="2" t="s">
+    </row>
+    <row r="23" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="14"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B22"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B6:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prototipo de interface e diagrama de estado do componente acessório completo
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
+++ b/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/DSS/Configura-Facil/diagramas/UseCases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20A2C50-6DAF-C34B-B48C-2112B394C11F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEC69E-FC02-2C4E-BFCF-4D322D3CB473}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>System response</t>
   </si>
@@ -67,58 +67,55 @@
     <t>1. Informa cancelamento do componente</t>
   </si>
   <si>
-    <t>4. Verifica necessidade de componentes extras</t>
-  </si>
-  <si>
-    <t>5.3. Retira componentes incompatíveis</t>
-  </si>
-  <si>
-    <t>5.2. Mantém componente atual</t>
-  </si>
-  <si>
-    <t>5.4 Retorna ao passo 5</t>
-  </si>
-  <si>
-    <t>5. Confirma compatibilidade com componentes escolhidos</t>
-  </si>
-  <si>
-    <t>5.1. Informa de incompatibilidade e apresenta os componentes incompatíveis</t>
-  </si>
-  <si>
-    <t>4.2. Confirma componentes extras</t>
-  </si>
-  <si>
-    <t>4.1. Informa de necessidade de mais componentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.3. Adiciona componentes extra </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alternativa 1 [Componente incompatível com existente]       Passo 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alternativa 2 [Necessita mais componentes] Passo 4</t>
-  </si>
-  <si>
     <t>Componente acessório selecionado</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>3. Apresenta preço do componente</t>
-  </si>
-  <si>
-    <t>6. Apresenta preço final</t>
-  </si>
-  <si>
-    <t>7. Confirma componte</t>
-  </si>
-  <si>
-    <t>8.  Adiciona componente</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Excepção 3 [Cliente não aceita componente] Passos 4.2, 5.2 e 7</t>
+    <t>3. Verifica necessidade de componentes extras</t>
+  </si>
+  <si>
+    <t>4. Confirma compatibilidade com componentes escolhidos</t>
+  </si>
+  <si>
+    <t>5. Apresenta preço final</t>
+  </si>
+  <si>
+    <t>6. Confirma componte</t>
+  </si>
+  <si>
+    <t>7.  Adiciona componente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternativa 1 [Componente incompatível com existente]       Passo 4</t>
+  </si>
+  <si>
+    <t>4.2. Mantém componente atual</t>
+  </si>
+  <si>
+    <t>4.1. Informa de incompatibilidade e apresenta os componentes incompatíveis</t>
+  </si>
+  <si>
+    <t>4.3. Retira componentes incompatíveis</t>
+  </si>
+  <si>
+    <t>4.4 Retorna ao passo 5</t>
+  </si>
+  <si>
+    <t>3.1. Informa de necessidade de mais componentes e apresenta os mesmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3. Adiciona componentes extra </t>
+  </si>
+  <si>
+    <t>3.2. Confirma componentes extras</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternativa 2 [Necessita mais componentes] Passo 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Excepção 3 [Cliente não aceita componente] Passos 3.2, 4.2 e 6</t>
   </si>
 </sst>
 </file>
@@ -757,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:G26"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +801,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D5" s="21"/>
     </row>
@@ -837,17 +834,17 @@
       <c r="B9" s="23"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B10" s="23"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="19" x14ac:dyDescent="0.25">
@@ -859,113 +856,106 @@
     </row>
     <row r="12" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B12" s="23"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B13" s="23"/>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="24"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="11" t="s">
-        <v>18</v>
-      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
-      <c r="C21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="2" t="s">
+    </row>
+    <row r="18" spans="2:4" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="17"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="14"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="14"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="B6:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revisão final dos diagramas
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
+++ b/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Use Case:</t>
   </si>
@@ -65,9 +65,6 @@
     <t xml:space="preserve">3. Verifica necessidade de componentes extras</t>
   </si>
   <si>
-    <t xml:space="preserve">s</t>
-  </si>
-  <si>
     <t xml:space="preserve">4. Confirma compatibilidade com componentes escolhidos</t>
   </si>
   <si>
@@ -80,7 +77,7 @@
     <t xml:space="preserve">7.  Adiciona componente acessório aos selecionados</t>
   </si>
   <si>
-    <t xml:space="preserve"> Alternativa 1 [Componente incompatível com outro já selecionado]  Passo 4</t>
+    <t xml:space="preserve"> Alternativa 1 [Componente incompatível com outro já selecionado]  (passo 4)</t>
   </si>
   <si>
     <t xml:space="preserve">4.1. Informa de incompatibilidades e apresenta os componentes incompatíveis</t>
@@ -95,7 +92,7 @@
     <t xml:space="preserve">4.4 Retorna ao passo 5</t>
   </si>
   <si>
-    <t xml:space="preserve"> Alternativa 2 [Necessita de componentes extra] Passo 3</t>
+    <t xml:space="preserve"> Alternativa 2 [Necessita de componentes extra] (passo 3)</t>
   </si>
   <si>
     <t xml:space="preserve">3.1. Informa de necessidade de mais componentes e apresenta-os</t>
@@ -107,7 +104,7 @@
     <t xml:space="preserve">3.3. Adiciona componentes extra </t>
   </si>
   <si>
-    <t xml:space="preserve"> Exceção 3 [Utilizador rejeita alterações] Passos 3.2, 4.2 e 6</t>
+    <t xml:space="preserve"> Exceção 3 [Utilizador rejeita alterações] (passos 3.2, 4.2 e 6)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Informa cancelamento do componente</t>
@@ -422,10 +419,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G1048576"/>
+  <dimension ref="B1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,34 +496,31 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4"/>
       <c r="C9" s="9"/>
       <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4"/>
       <c r="C10" s="9"/>
       <c r="D10" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4"/>
       <c r="C11" s="9"/>
       <c r="D11" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4"/>
       <c r="C12" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="8"/>
     </row>
@@ -534,7 +528,7 @@
       <c r="B13" s="4"/>
       <c r="C13" s="9"/>
       <c r="D13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,17 +538,17 @@
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="12"/>
       <c r="C16" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="8"/>
     </row>
@@ -562,29 +556,29 @@
       <c r="B17" s="12"/>
       <c r="C17" s="9"/>
       <c r="D17" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="12"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="15"/>
       <c r="C20" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="8"/>
     </row>
@@ -592,16 +586,16 @@
       <c r="B21" s="15"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -614,7 +608,6 @@
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="1048576" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C2:D2"/>

</xml_diff>

<commit_message>
DSS de Componentes Acessórios feito
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
+++ b/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/DSS/Configura-Facil/diagramas/UseCases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BED8BA-7250-446D-B49D-FCE71BCF2EF1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3152CCDE-67FC-AC42-BD69-65765FD1D38C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Use Case:</t>
   </si>
@@ -61,9 +61,6 @@
     <t>System response</t>
   </si>
   <si>
-    <t>1. Apresenta lista de componentes</t>
-  </si>
-  <si>
     <t>2. Seleciona componente</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>4.3. Retira componentes incompatíveis</t>
   </si>
   <si>
-    <t>4.4 Retorna ao passo 5</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Alternativa 2 [Necessita de componentes extra] (passo 3)</t>
   </si>
   <si>
@@ -113,6 +107,9 @@
   </si>
   <si>
     <t>1. Informa cancelamento do componente</t>
+  </si>
+  <si>
+    <t>1. Apresenta lista de componentes acessórios</t>
   </si>
 </sst>
 </file>
@@ -304,21 +301,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,6 +319,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,199 +717,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
-    <col min="4" max="4" width="74.625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="74.6640625" customWidth="1"/>
     <col min="5" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10" t="s">
+    <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B9" s="16"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10" t="s">
+    </row>
+    <row r="10" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10" t="s">
+    <row r="11" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10" t="s">
+    <row r="12" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10" t="s">
+    </row>
+    <row r="14" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="16" t="s">
+    </row>
+    <row r="16" spans="2:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="2:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10" t="s">
+    </row>
+    <row r="18" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="2:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13"/>
+      <c r="C19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="2:4" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="13"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
+    <row r="21" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="2:4" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="2:4" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
+    <row r="22" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="2:4" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>

<commit_message>
Pequena alteração no DSS acessório
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
+++ b/diagramas/UseCases/EscolherComponenteAcessorio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/DSS/Configura-Facil/diagramas/UseCases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3152CCDE-67FC-AC42-BD69-65765FD1D38C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A92EA2E-7E90-C340-8577-CCB665800C14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>2. Seleciona componente</t>
   </si>
   <si>
-    <t>3. Verifica necessidade de componentes extras</t>
-  </si>
-  <si>
     <t>4. Confirma compatibilidade com componentes escolhidos</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>1. Apresenta lista de componentes acessórios</t>
+  </si>
+  <si>
+    <t>3. Verifica necessidade de componentes extra</t>
   </si>
 </sst>
 </file>
@@ -720,7 +720,7 @@
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,7 +783,7 @@
       <c r="B7" s="16"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19" x14ac:dyDescent="0.25">
@@ -797,27 +797,27 @@
       <c r="B9" s="16"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="6"/>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
       <c r="C11" s="6"/>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B12" s="16"/>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -825,7 +825,7 @@
       <c r="B13" s="16"/>
       <c r="C13" s="6"/>
       <c r="D13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19" x14ac:dyDescent="0.25">
@@ -835,17 +835,17 @@
     </row>
     <row r="15" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -853,22 +853,22 @@
       <c r="B17" s="12"/>
       <c r="C17" s="6"/>
       <c r="D17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13"/>
       <c r="C19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -876,16 +876,16 @@
       <c r="B20" s="13"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="37" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>